<commit_message>
Disable SRB1; change 0xF1 to 0xE1.
</commit_message>
<xml_diff>
--- a/Ads1299_defRegs.xlsx
+++ b/Ads1299_defRegs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahmood31\Google Drive\nRF5_SDK_13.1.0\examples\_my_projects\nRF52_ADS1299_ExG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahmood31\Google Drive\nRF5_SDK_13.1.0\examples\_my_projects\nRF52_ADS1299_ExG_MPU9250\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -712,7 +712,7 @@
   <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,31 +1005,31 @@
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>0x60</v>
-      </c>
-      <c r="D7" s="14">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4">
-        <v>1</v>
-      </c>
-      <c r="F7" s="4">
-        <v>1</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0</v>
-      </c>
-      <c r="H7" s="7">
-        <v>0</v>
-      </c>
-      <c r="I7" s="4">
-        <v>0</v>
-      </c>
-      <c r="J7" s="4">
-        <v>0</v>
-      </c>
-      <c r="K7" s="4">
-        <v>0</v>
+        <v>0xE1</v>
+      </c>
+      <c r="D7" s="11">
+        <v>1</v>
+      </c>
+      <c r="E7" s="11">
+        <v>1</v>
+      </c>
+      <c r="F7" s="11">
+        <v>1</v>
+      </c>
+      <c r="G7" s="11">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0</v>
+      </c>
+      <c r="I7" s="11">
+        <v>0</v>
+      </c>
+      <c r="J7" s="11">
+        <v>0</v>
+      </c>
+      <c r="K7" s="11">
+        <v>1</v>
       </c>
       <c r="L7" s="4">
         <v>49</v>
@@ -1044,31 +1044,31 @@
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>0x60</v>
-      </c>
-      <c r="D8" s="14">
-        <v>0</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0</v>
-      </c>
-      <c r="H8" s="7">
-        <v>0</v>
-      </c>
-      <c r="I8" s="4">
-        <v>0</v>
-      </c>
-      <c r="J8" s="4">
-        <v>0</v>
-      </c>
-      <c r="K8" s="4">
-        <v>0</v>
+        <v>0xE1</v>
+      </c>
+      <c r="D8" s="11">
+        <v>1</v>
+      </c>
+      <c r="E8" s="11">
+        <v>1</v>
+      </c>
+      <c r="F8" s="11">
+        <v>1</v>
+      </c>
+      <c r="G8" s="11">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0</v>
+      </c>
+      <c r="I8" s="11">
+        <v>0</v>
+      </c>
+      <c r="J8" s="11">
+        <v>0</v>
+      </c>
+      <c r="K8" s="11">
+        <v>1</v>
       </c>
       <c r="L8" s="4">
         <v>49</v>
@@ -1083,31 +1083,31 @@
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v>0x60</v>
-      </c>
-      <c r="D9" s="14">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1</v>
-      </c>
-      <c r="F9" s="4">
-        <v>1</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0</v>
-      </c>
-      <c r="H9" s="7">
-        <v>0</v>
-      </c>
-      <c r="I9" s="4">
-        <v>0</v>
-      </c>
-      <c r="J9" s="4">
-        <v>0</v>
-      </c>
-      <c r="K9" s="4">
-        <v>0</v>
+        <v>0xE1</v>
+      </c>
+      <c r="D9" s="11">
+        <v>1</v>
+      </c>
+      <c r="E9" s="11">
+        <v>1</v>
+      </c>
+      <c r="F9" s="11">
+        <v>1</v>
+      </c>
+      <c r="G9" s="11">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11">
+        <v>0</v>
+      </c>
+      <c r="I9" s="11">
+        <v>0</v>
+      </c>
+      <c r="J9" s="11">
+        <v>0</v>
+      </c>
+      <c r="K9" s="11">
+        <v>1</v>
       </c>
       <c r="L9" s="4">
         <v>49</v>
@@ -1122,7 +1122,7 @@
       </c>
       <c r="C10" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0xF1</v>
+        <v>0xE1</v>
       </c>
       <c r="D10" s="11">
         <v>1</v>
@@ -1134,7 +1134,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="11">
         <v>0</v>
@@ -1164,7 +1164,7 @@
       </c>
       <c r="C11" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0xF1</v>
+        <v>0xE1</v>
       </c>
       <c r="D11" s="11">
         <v>1</v>
@@ -1176,7 +1176,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" s="11">
         <v>0</v>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="C12" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0xF1</v>
+        <v>0xE1</v>
       </c>
       <c r="D12" s="11">
         <v>1</v>
@@ -1215,7 +1215,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" s="11">
         <v>0</v>
@@ -1242,7 +1242,7 @@
       </c>
       <c r="C13" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0xF1</v>
+        <v>0xE1</v>
       </c>
       <c r="D13" s="11">
         <v>1</v>
@@ -1254,7 +1254,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" s="11">
         <v>0</v>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
-        <v>0x20</v>
+        <v>0x00</v>
       </c>
       <c r="D22" s="6">
         <v>0</v>
@@ -1620,7 +1620,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" s="6">
         <v>0</v>

</xml_diff>

<commit_message>
Everything works finally with acceptable throughput using a 9-byte SPI buffer and a 240-byte BLE buffer. Throughput is an acceptable 24kB/s with very minor deviations.
</commit_message>
<xml_diff>
--- a/Ads1299_defRegs.xlsx
+++ b/Ads1299_defRegs.xlsx
@@ -711,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,7 +822,7 @@
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C24" si="0">"0x"&amp;TEXT(DEC2HEX(K3+2*J3+4*I3+8*H3+16*G3+32*F3+64*E3+128*D3,2),"00")</f>
-        <v>0xD2</v>
+        <v>0xD1</v>
       </c>
       <c r="D3" s="6">
         <v>1</v>
@@ -833,7 +833,7 @@
       <c r="F3" s="6">
         <v>0</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>1</v>
       </c>
       <c r="H3" s="6">
@@ -843,10 +843,10 @@
         <v>0</v>
       </c>
       <c r="J3" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3" s="4">
         <v>46</v>
@@ -912,7 +912,7 @@
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v>0x02</v>
+        <v>0x00</v>
       </c>
       <c r="D5" s="4">
         <v>0</v>
@@ -933,7 +933,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" s="7">
         <v>0</v>
@@ -1044,7 +1044,7 @@
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>0xE1</v>
+        <v>0xE5</v>
       </c>
       <c r="D8" s="11">
         <v>1</v>
@@ -1062,7 +1062,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="11">
         <v>0</v>

</xml_diff>

<commit_message>
High-fidelity test signal throughput at 8kHz. Uses workaround that checks last 12 bits of data. If it is equal to 0, it ignores the transfer.
</commit_message>
<xml_diff>
--- a/Ads1299_defRegs.xlsx
+++ b/Ads1299_defRegs.xlsx
@@ -711,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,7 +777,7 @@
       </c>
       <c r="C2" t="str">
         <f>"0x"&amp;TEXT(DEC2HEX(K2+2*J2+4*I2+8*H2+16*G2+32*F2+64*E2+128*D2,2),"00")</f>
-        <v>0x96</v>
+        <v>0x91</v>
       </c>
       <c r="D2" s="6">
         <v>1</v>
@@ -795,13 +795,13 @@
         <v>0</v>
       </c>
       <c r="I2" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" s="4">
         <v>45</v>
@@ -822,7 +822,7 @@
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C24" si="0">"0x"&amp;TEXT(DEC2HEX(K3+2*J3+4*I3+8*H3+16*G3+32*F3+64*E3+128*D3,2),"00")</f>
-        <v>0xD1</v>
+        <v>0xD3</v>
       </c>
       <c r="D3" s="6">
         <v>1</v>
@@ -843,7 +843,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" s="8">
         <v>1</v>
@@ -1044,10 +1044,10 @@
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>0xE5</v>
+        <v>0x65</v>
       </c>
       <c r="D8" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="11">
         <v>1</v>

</xml_diff>

<commit_message>
Removed temp workaround and now everything seems to work fine.
</commit_message>
<xml_diff>
--- a/Ads1299_defRegs.xlsx
+++ b/Ads1299_defRegs.xlsx
@@ -712,7 +712,7 @@
   <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,10 +1005,10 @@
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>0xE1</v>
+        <v>0x61</v>
       </c>
       <c r="D7" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="11">
         <v>1</v>

</xml_diff>